<commit_message>
R403, 404, 405 corrected
</commit_message>
<xml_diff>
--- a/rotating_sphere_electronics/RS64c/production/bom.xlsx
+++ b/rotating_sphere_electronics/RS64c/production/bom.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ludwin/Elektronik/rotating_sphere/rotating_sphere_electronics/RS64c/production/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF65308F-4D34-E342-83AE-3A1943879456}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56E57B57-C90D-E044-842D-0EA91DF7047A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11700" yWindow="980" windowWidth="10000" windowHeight="16980" xr2:uid="{AEECF7DE-BEF7-2F45-88BA-D920ADAADBEA}"/>
+    <workbookView xWindow="140" yWindow="840" windowWidth="28480" windowHeight="17640" xr2:uid="{AEECF7DE-BEF7-2F45-88BA-D920ADAADBEA}"/>
   </bookViews>
   <sheets>
     <sheet name="bom" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="95">
   <si>
     <t>Designator</t>
   </si>
@@ -302,6 +302,9 @@
   </si>
   <si>
     <t>C9002</t>
+  </si>
+  <si>
+    <t>C25099</t>
   </si>
 </sst>
 </file>
@@ -1165,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16A8F76-CD21-1547-B0C3-D4842F013CCD}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="99" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1412,7 +1415,7 @@
         <v>54</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>41</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>